<commit_message>
Update TFV mapping keys
</commit_message>
<xml_diff>
--- a/scripting/boundary_conditions/wlwq_allsamples/TFV_mapping_keys.xlsx
+++ b/scripting/boundary_conditions/wlwq_allsamples/TFV_mapping_keys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassie-lake/tassielakes-data/scripting/boundary_conditions/wlwq_allsamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3252B7-1DD8-7B4B-9221-D51DF6CBCD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5231A83-9F11-C34D-86A8-E30A272EDA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14660" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{31442990-50AF-C843-98D9-B85B28910463}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="554">
   <si>
     <t>Params.Name</t>
   </si>
@@ -1694,13 +1694,16 @@
   </si>
   <si>
     <t>1992-2011</t>
+  </si>
+  <si>
+    <t>MARVL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1848,8 +1851,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2049,18 +2059,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2226,14 +2224,25 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2615,1418 +2624,1455 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" style="7"/>
     <col min="3" max="3" width="39.5" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="47.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="47.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>520</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>521</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>522</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>524</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>525</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="J2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="5">
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="5">
         <v>32.258064516129032</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="J7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="5">
         <v>31.25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="5">
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="5">
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>485</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="5">
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="4">
         <v>100.0869</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="5" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="J15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="J15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="J16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="J16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="J17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="5">
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="J19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="4">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
-      <c r="K20" s="4" t="s">
+      <c r="J20" s="5">
+        <v>1</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="4">
-        <v>1</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J21" s="1">
-        <v>1</v>
-      </c>
-      <c r="K21" s="4" t="s">
+      <c r="J21" s="5">
+        <v>1</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J22" s="1">
-        <v>1</v>
-      </c>
-      <c r="K22" s="4" t="s">
+      <c r="J22" s="5">
+        <v>1</v>
+      </c>
+      <c r="K22" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="4">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5" t="s">
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J23" s="1">
-        <v>1</v>
-      </c>
-      <c r="K23" s="4" t="s">
+      <c r="J23" s="5">
+        <v>1</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="5" t="s">
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J24" s="1">
-        <v>1</v>
-      </c>
-      <c r="K24" s="4" t="s">
+      <c r="J24" s="5">
+        <v>1</v>
+      </c>
+      <c r="K24" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="5" t="s">
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J25" s="1">
-        <v>1</v>
-      </c>
-      <c r="K25" s="4" t="s">
+      <c r="J25" s="5">
+        <v>1</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>550</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
-      <c r="G26" s="5" t="s">
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J26" s="1">
-        <v>1</v>
-      </c>
-      <c r="K26" s="4" t="s">
+      <c r="J26" s="5">
+        <v>1</v>
+      </c>
+      <c r="K26" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4" t="s">
+      <c r="E27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="H27" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27" s="4" t="s">
+      <c r="J27" s="5">
+        <v>1</v>
+      </c>
+      <c r="K27" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
         <v>2004</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="5" t="s">
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J28" s="1">
-        <v>1</v>
-      </c>
-      <c r="K28" s="4" t="s">
+      <c r="J28" s="5">
+        <v>1</v>
+      </c>
+      <c r="K28" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="4">
-        <v>1</v>
-      </c>
-      <c r="G29" s="5" t="s">
+      <c r="F29" s="5">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J29" s="1">
-        <v>1</v>
-      </c>
-      <c r="K29" s="4" t="s">
+      <c r="J29" s="5">
+        <v>1</v>
+      </c>
+      <c r="K29" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="4">
-        <v>1</v>
-      </c>
-      <c r="G30" s="5" t="s">
+      <c r="F30" s="5">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J30" s="1">
-        <v>1</v>
-      </c>
-      <c r="K30" s="4" t="s">
+      <c r="J30" s="5">
+        <v>1</v>
+      </c>
+      <c r="K30" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="4">
-        <v>1</v>
-      </c>
-      <c r="G31" s="5" t="s">
+      <c r="F31" s="5">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I31" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J31" s="1">
-        <v>1</v>
-      </c>
-      <c r="K31" s="4" t="s">
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
         <v>2012</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="4">
-        <v>1</v>
-      </c>
-      <c r="G32" s="5" t="s">
+      <c r="F32" s="5">
+        <v>1</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>503</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I32" s="1" t="s">
+      <c r="H32" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J32" s="1">
-        <v>1</v>
-      </c>
-      <c r="K32" s="4" t="s">
+      <c r="J32" s="5">
+        <v>1</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
         <v>2012</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="4">
-        <v>1</v>
-      </c>
-      <c r="G33" s="5" t="s">
+      <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I33" s="1" t="s">
+      <c r="H33" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J33" s="1">
-        <v>1</v>
-      </c>
-      <c r="K33" s="4" t="s">
+      <c r="J33" s="5">
+        <v>1</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="4">
-        <v>1</v>
-      </c>
-      <c r="G34" s="4" t="s">
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>505</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I34" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J34" s="1">
-        <v>1</v>
-      </c>
-      <c r="K34" s="4" t="s">
+      <c r="J34" s="5">
+        <v>1</v>
+      </c>
+      <c r="K34" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
         <v>2014</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="4" t="s">
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I35" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J35" s="1">
-        <v>1</v>
-      </c>
-      <c r="K35" s="4" t="s">
+      <c r="J35" s="5">
+        <v>1</v>
+      </c>
+      <c r="K35" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="4">
-        <v>1</v>
-      </c>
-      <c r="G36" s="4" t="s">
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I36" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J36" s="1">
-        <v>1</v>
-      </c>
-      <c r="K36" s="4" t="s">
+      <c r="J36" s="5">
+        <v>1</v>
+      </c>
+      <c r="K36" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="F37" s="4">
-        <v>1</v>
-      </c>
-      <c r="G37" s="4" t="s">
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="J37" s="6">
+      <c r="J37" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="F38" s="5">
+        <v>1</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I38" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="5">
         <v>32.258064516129032</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
         <v>552</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="1">
-        <v>1</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="F39" s="5">
+        <v>1</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I39" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="5">
         <v>32.258064516129032</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="K39" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="1">
-        <v>1</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I40" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="J40" s="6">
+      <c r="J40" s="4">
         <v>96.06</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="M40" s="4" t="s">
+      <c r="K40" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="M40" s="5" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="F41" s="5">
+        <v>1</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I41" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="J41" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="J41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="F42" s="1">
-        <v>1</v>
-      </c>
-      <c r="G42" s="4" t="s">
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I42" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="J42" s="1">
-        <v>1</v>
-      </c>
+      <c r="J42" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>

<commit_message>
Update swift inflow data
</commit_message>
<xml_diff>
--- a/scripting/boundary_conditions/wlwq_allsamples/TFV_mapping_keys.xlsx
+++ b/scripting/boundary_conditions/wlwq_allsamples/TFV_mapping_keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassie-lake/tassielakes-data/scripting/boundary_conditions/wlwq_allsamples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/scripting/boundary_conditions/wlwq_allsamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363B0035-7FED-9449-A394-6BAEAFCDE6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592206EC-E8E7-6B48-9F0D-81416DCA93B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="14700" windowHeight="17200" xr2:uid="{31442990-50AF-C843-98D9-B85B28910463}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="17200" activeTab="1" xr2:uid="{31442990-50AF-C843-98D9-B85B28910463}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_TFV_Y" sheetId="3" r:id="rId1"/>
@@ -1792,12 +1792,6 @@
     <t>WQ_DIAG_PHY_CHARA_ZYGNEMA</t>
   </si>
   <si>
-    <t>WQ_DIAG_PHY_GRN__ANKISTRODESMUS</t>
-  </si>
-  <si>
-    <t>WQ_DIAG_PHY_GRN__ANKYRA</t>
-  </si>
-  <si>
     <t>WQ_DIAG_PHY_GRN_BOTRYCOCCUS</t>
   </si>
   <si>
@@ -2123,6 +2117,12 @@
   </si>
   <si>
     <t>AIR_TEMPERATURE</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_ANKISTRODESMUS</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_GRN_ANKYRA</t>
   </si>
 </sst>
 </file>
@@ -2285,7 +2285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2491,7 +2491,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDAF2D0"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -2656,7 +2662,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2671,7 +2677,8 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3052,7 +3059,7 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D20" sqref="D20:D37"/>
     </sheetView>
   </sheetViews>
@@ -3409,7 +3416,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H11" t="s">
         <v>10</v>
@@ -3569,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H16" t="s">
         <v>43</v>
@@ -4480,8 +4487,8 @@
   </sheetPr>
   <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4524,10 +4531,10 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="10" t="s">
         <v>135</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -4553,10 +4560,10 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>137</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -4582,10 +4589,10 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="10" t="s">
         <v>139</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -4611,13 +4618,13 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="10" t="s">
         <v>556</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -4640,13 +4647,13 @@
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="10" t="s">
         <v>557</v>
       </c>
       <c r="G6" s="3">
@@ -4669,13 +4676,13 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="10" t="s">
         <v>558</v>
       </c>
       <c r="G7" s="3">
@@ -4698,13 +4705,13 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="10" t="s">
         <v>559</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -4727,13 +4734,13 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="10" t="s">
         <v>560</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -4756,13 +4763,13 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="10" t="s">
         <v>561</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -4785,13 +4792,13 @@
       <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="10" t="s">
         <v>562</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -4814,13 +4821,13 @@
       <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="10" t="s">
         <v>563</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -4843,13 +4850,13 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="10" t="s">
         <v>564</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -4872,13 +4879,13 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="10" t="s">
         <v>565</v>
       </c>
       <c r="G14" s="3">
@@ -4901,13 +4908,13 @@
       <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="10" t="s">
         <v>566</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -4922,7 +4929,7 @@
     </row>
     <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E16" s="3" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>519</v>
@@ -4938,13 +4945,13 @@
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="10" t="s">
         <v>576</v>
       </c>
       <c r="H17" s="3" t="s">
@@ -4964,13 +4971,13 @@
       <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="10" t="s">
         <v>577</v>
       </c>
       <c r="H18" s="3" t="s">
@@ -4990,13 +4997,13 @@
       <c r="C19" s="3">
         <v>1</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="10" t="s">
         <v>578</v>
       </c>
       <c r="H19" s="3" t="s">
@@ -5016,13 +5023,13 @@
       <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="10" t="s">
         <v>579</v>
       </c>
       <c r="H20" s="3" t="s">
@@ -5042,13 +5049,13 @@
       <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="10" t="s">
         <v>580</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -5068,13 +5075,13 @@
       <c r="C22" s="3">
         <v>1</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="10" t="s">
         <v>581</v>
       </c>
       <c r="H22" s="3" t="s">
@@ -5094,13 +5101,13 @@
       <c r="C23" s="3">
         <v>1</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="10" t="s">
         <v>582</v>
       </c>
       <c r="H23" s="3" t="s">
@@ -5120,13 +5127,13 @@
       <c r="C24" s="3">
         <v>1</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="10" t="s">
         <v>583</v>
       </c>
       <c r="H24" s="3" t="s">
@@ -5146,13 +5153,13 @@
       <c r="C25" s="3">
         <v>1</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="10" t="s">
         <v>584</v>
       </c>
       <c r="H25" s="3" t="s">
@@ -5164,10 +5171,10 @@
     </row>
     <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E26" s="3" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -5180,14 +5187,14 @@
       <c r="C27" s="3">
         <v>1</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>585</v>
+      <c r="F27" s="10" t="s">
+        <v>694</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>130</v>
@@ -5206,14 +5213,14 @@
       <c r="C28" s="3">
         <v>1</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>586</v>
+      <c r="F28" s="10" t="s">
+        <v>695</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>130</v>
@@ -5232,14 +5239,14 @@
       <c r="C29" s="3">
         <v>1</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>587</v>
+      <c r="F29" s="10" t="s">
+        <v>585</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>130</v>
@@ -5258,14 +5265,14 @@
       <c r="C30" s="3">
         <v>1</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>588</v>
+      <c r="F30" s="10" t="s">
+        <v>586</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>130</v>
@@ -5284,14 +5291,14 @@
       <c r="C31" s="3">
         <v>1</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>589</v>
+      <c r="F31" s="10" t="s">
+        <v>587</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>130</v>
@@ -5310,14 +5317,14 @@
       <c r="C32" s="3">
         <v>1</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>590</v>
+      <c r="F32" s="10" t="s">
+        <v>588</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>130</v>
@@ -5336,14 +5343,14 @@
       <c r="C33" s="3">
         <v>1</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>591</v>
+      <c r="F33" s="10" t="s">
+        <v>589</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>130</v>
@@ -5362,14 +5369,14 @@
       <c r="C34" s="3">
         <v>1</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>592</v>
+      <c r="F34" s="10" t="s">
+        <v>590</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>130</v>
@@ -5388,14 +5395,14 @@
       <c r="C35" s="3">
         <v>1</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>593</v>
+      <c r="F35" s="10" t="s">
+        <v>591</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>130</v>
@@ -5414,14 +5421,14 @@
       <c r="C36" s="3">
         <v>1</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>594</v>
+      <c r="F36" s="10" t="s">
+        <v>592</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>130</v>
@@ -5440,14 +5447,14 @@
       <c r="C37" s="3">
         <v>1</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>595</v>
+      <c r="F37" s="10" t="s">
+        <v>593</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>130</v>
@@ -5466,14 +5473,14 @@
       <c r="C38" s="3">
         <v>1</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>596</v>
+      <c r="F38" s="10" t="s">
+        <v>594</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>130</v>
@@ -5492,14 +5499,14 @@
       <c r="C39" s="3">
         <v>1</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>597</v>
+      <c r="F39" s="10" t="s">
+        <v>595</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>130</v>
@@ -5518,14 +5525,14 @@
       <c r="C40" s="3">
         <v>1</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>598</v>
+      <c r="F40" s="10" t="s">
+        <v>596</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>130</v>
@@ -5544,14 +5551,14 @@
       <c r="C41" s="3">
         <v>1</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>599</v>
+      <c r="F41" s="10" t="s">
+        <v>597</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>130</v>
@@ -5570,14 +5577,14 @@
       <c r="C42" s="3">
         <v>1</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>600</v>
+      <c r="F42" s="10" t="s">
+        <v>598</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>130</v>
@@ -5596,14 +5603,14 @@
       <c r="C43" s="3">
         <v>1</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>601</v>
+      <c r="F43" s="10" t="s">
+        <v>599</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>130</v>
@@ -5622,14 +5629,14 @@
       <c r="C44" s="3">
         <v>1</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>602</v>
+      <c r="F44" s="10" t="s">
+        <v>600</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>130</v>
@@ -5648,14 +5655,14 @@
       <c r="C45" s="3">
         <v>1</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>603</v>
+      <c r="F45" s="10" t="s">
+        <v>601</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>130</v>
@@ -5674,14 +5681,14 @@
       <c r="C46" s="3">
         <v>1</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>604</v>
+      <c r="F46" s="10" t="s">
+        <v>602</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>130</v>
@@ -5700,14 +5707,14 @@
       <c r="C47" s="3">
         <v>1</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>605</v>
+      <c r="F47" s="10" t="s">
+        <v>603</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>130</v>
@@ -5726,14 +5733,14 @@
       <c r="C48" s="3">
         <v>1</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>606</v>
+      <c r="F48" s="10" t="s">
+        <v>604</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>130</v>
@@ -5752,14 +5759,14 @@
       <c r="C49" s="3">
         <v>1</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>607</v>
+      <c r="F49" s="10" t="s">
+        <v>605</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>130</v>
@@ -5778,14 +5785,14 @@
       <c r="C50" s="3">
         <v>1</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>608</v>
+      <c r="F50" s="10" t="s">
+        <v>606</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>130</v>
@@ -5804,14 +5811,14 @@
       <c r="C51" s="3">
         <v>1</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>609</v>
+      <c r="F51" s="10" t="s">
+        <v>607</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>130</v>
@@ -5830,14 +5837,14 @@
       <c r="C52" s="3">
         <v>1</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>610</v>
+      <c r="F52" s="10" t="s">
+        <v>608</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>130</v>
@@ -5856,14 +5863,14 @@
       <c r="C53" s="3">
         <v>1</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>611</v>
+      <c r="F53" s="10" t="s">
+        <v>609</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>130</v>
@@ -5882,14 +5889,14 @@
       <c r="C54" s="3">
         <v>1</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>612</v>
+      <c r="F54" s="10" t="s">
+        <v>610</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>130</v>
@@ -5908,14 +5915,14 @@
       <c r="C55" s="3">
         <v>1</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>613</v>
+      <c r="F55" s="10" t="s">
+        <v>611</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>130</v>
@@ -5934,14 +5941,14 @@
       <c r="C56" s="3">
         <v>1</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>614</v>
+      <c r="F56" s="10" t="s">
+        <v>612</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>130</v>
@@ -5960,14 +5967,14 @@
       <c r="C57" s="3">
         <v>1</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>615</v>
+      <c r="F57" s="10" t="s">
+        <v>613</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>130</v>
@@ -5986,14 +5993,14 @@
       <c r="C58" s="3">
         <v>1</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>616</v>
+      <c r="F58" s="10" t="s">
+        <v>614</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>130</v>
@@ -6012,14 +6019,14 @@
       <c r="C59" s="3">
         <v>1</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>617</v>
+      <c r="F59" s="10" t="s">
+        <v>615</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>130</v>
@@ -6038,14 +6045,14 @@
       <c r="C60" s="3">
         <v>1</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>618</v>
+      <c r="F60" s="10" t="s">
+        <v>616</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>130</v>
@@ -6064,14 +6071,14 @@
       <c r="C61" s="3">
         <v>1</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>619</v>
+      <c r="F61" s="10" t="s">
+        <v>617</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>130</v>
@@ -6090,14 +6097,14 @@
       <c r="C62" s="3">
         <v>1</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>620</v>
+      <c r="F62" s="10" t="s">
+        <v>618</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>130</v>
@@ -6116,14 +6123,14 @@
       <c r="C63" s="3">
         <v>1</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>621</v>
+      <c r="F63" s="10" t="s">
+        <v>619</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>130</v>
@@ -6142,14 +6149,14 @@
       <c r="C64" s="3">
         <v>1</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>622</v>
+      <c r="F64" s="10" t="s">
+        <v>620</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>130</v>
@@ -6168,14 +6175,14 @@
       <c r="C65" s="3">
         <v>1</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>623</v>
+      <c r="F65" s="10" t="s">
+        <v>621</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>130</v>
@@ -6194,14 +6201,14 @@
       <c r="C66" s="3">
         <v>1</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>624</v>
+      <c r="F66" s="10" t="s">
+        <v>622</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>130</v>
@@ -6220,14 +6227,14 @@
       <c r="C67" s="3">
         <v>1</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>625</v>
+      <c r="F67" s="10" t="s">
+        <v>623</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>130</v>
@@ -6246,14 +6253,14 @@
       <c r="C68" s="3">
         <v>1</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>626</v>
+      <c r="F68" s="10" t="s">
+        <v>624</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>130</v>
@@ -6264,10 +6271,10 @@
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E69" s="3" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -6280,14 +6287,14 @@
       <c r="C70" s="3">
         <v>1</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>630</v>
+      <c r="F70" s="10" t="s">
+        <v>628</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>130</v>
@@ -6306,14 +6313,14 @@
       <c r="C71" s="3">
         <v>1</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>631</v>
+      <c r="F71" s="10" t="s">
+        <v>629</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>130</v>
@@ -6332,14 +6339,14 @@
       <c r="C72" s="3">
         <v>1</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>632</v>
+      <c r="F72" s="10" t="s">
+        <v>630</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>130</v>
@@ -6358,14 +6365,14 @@
       <c r="C73" s="3">
         <v>1</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>633</v>
+      <c r="F73" s="10" t="s">
+        <v>631</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>130</v>
@@ -6384,14 +6391,14 @@
       <c r="C74" s="3">
         <v>1</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>634</v>
+      <c r="F74" s="10" t="s">
+        <v>632</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>130</v>
@@ -6402,10 +6409,10 @@
     </row>
     <row r="75" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E75" s="3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -6418,14 +6425,14 @@
       <c r="C76" s="3">
         <v>1</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E76" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>635</v>
+      <c r="F76" s="10" t="s">
+        <v>633</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>130</v>
@@ -6444,14 +6451,14 @@
       <c r="C77" s="3">
         <v>1</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="F77" s="3" t="s">
-        <v>636</v>
+      <c r="F77" s="10" t="s">
+        <v>634</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>130</v>
@@ -6470,14 +6477,14 @@
       <c r="C78" s="3">
         <v>1</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>637</v>
+      <c r="F78" s="10" t="s">
+        <v>635</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>130</v>
@@ -6488,10 +6495,10 @@
     </row>
     <row r="79" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E79" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -6504,14 +6511,14 @@
       <c r="C80" s="3">
         <v>1</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D80" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E80" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="F80" s="3" t="s">
-        <v>639</v>
+      <c r="F80" s="10" t="s">
+        <v>637</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>130</v>
@@ -6530,14 +6537,14 @@
       <c r="C81" s="3">
         <v>1</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D81" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E81" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>640</v>
+      <c r="F81" s="10" t="s">
+        <v>638</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>130</v>
@@ -6556,14 +6563,14 @@
       <c r="C82" s="3">
         <v>1</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E82" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>641</v>
+      <c r="F82" s="10" t="s">
+        <v>639</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>130</v>
@@ -6582,14 +6589,14 @@
       <c r="C83" s="3">
         <v>1</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D83" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E83" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>642</v>
+      <c r="F83" s="10" t="s">
+        <v>640</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>130</v>
@@ -6608,14 +6615,14 @@
       <c r="C84" s="3">
         <v>1</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D84" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E84" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>643</v>
+      <c r="F84" s="10" t="s">
+        <v>641</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>130</v>
@@ -6634,14 +6641,14 @@
       <c r="C85" s="3">
         <v>1</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="E85" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="F85" s="3" t="s">
-        <v>644</v>
+      <c r="F85" s="10" t="s">
+        <v>642</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>130</v>
@@ -6660,14 +6667,14 @@
       <c r="C86" s="3">
         <v>1</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="E86" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>645</v>
+      <c r="F86" s="10" t="s">
+        <v>643</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>130</v>
@@ -6686,14 +6693,14 @@
       <c r="C87" s="3">
         <v>1</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="E87" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>646</v>
+      <c r="F87" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>130</v>
@@ -6712,14 +6719,14 @@
       <c r="C88" s="3">
         <v>1</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="E88" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>647</v>
+      <c r="F88" s="10" t="s">
+        <v>645</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>130</v>
@@ -6738,14 +6745,14 @@
       <c r="C89" s="3">
         <v>1</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="10" t="s">
         <v>321</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E89" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>648</v>
+      <c r="F89" s="10" t="s">
+        <v>646</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>130</v>
@@ -6764,14 +6771,14 @@
       <c r="C90" s="3">
         <v>1</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E90" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>649</v>
+      <c r="F90" s="10" t="s">
+        <v>647</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>130</v>
@@ -6790,14 +6797,14 @@
       <c r="C91" s="3">
         <v>1</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E91" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="F91" s="3" t="s">
-        <v>650</v>
+      <c r="F91" s="10" t="s">
+        <v>648</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>130</v>
@@ -6816,14 +6823,14 @@
       <c r="C92" s="3">
         <v>1</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E92" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>651</v>
+      <c r="F92" s="10" t="s">
+        <v>649</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>130</v>
@@ -6842,14 +6849,14 @@
       <c r="C93" s="3">
         <v>1</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E93" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="F93" s="3" t="s">
-        <v>652</v>
+      <c r="F93" s="10" t="s">
+        <v>650</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>130</v>
@@ -6868,14 +6875,14 @@
       <c r="C94" s="3">
         <v>1</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="E94" s="3" t="s">
-        <v>654</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>653</v>
+      <c r="E94" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>651</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>130</v>
@@ -6894,14 +6901,14 @@
       <c r="C95" s="3">
         <v>1</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E95" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>655</v>
+      <c r="F95" s="10" t="s">
+        <v>653</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>130</v>
@@ -6920,14 +6927,14 @@
       <c r="C96" s="3">
         <v>1</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E96" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="F96" s="3" t="s">
-        <v>656</v>
+      <c r="F96" s="10" t="s">
+        <v>654</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>130</v>
@@ -6946,14 +6953,14 @@
       <c r="C97" s="3">
         <v>1</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D97" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E97" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>657</v>
+      <c r="F97" s="10" t="s">
+        <v>655</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>130</v>
@@ -6972,14 +6979,14 @@
       <c r="C98" s="3">
         <v>1</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D98" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E98" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>658</v>
+      <c r="F98" s="10" t="s">
+        <v>656</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>130</v>
@@ -6998,14 +7005,14 @@
       <c r="C99" s="3">
         <v>1</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D99" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E99" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>659</v>
+      <c r="F99" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>130</v>
@@ -7024,14 +7031,14 @@
       <c r="C100" s="3">
         <v>1</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E100" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F100" s="3" t="s">
-        <v>660</v>
+      <c r="F100" s="10" t="s">
+        <v>658</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>130</v>
@@ -7050,14 +7057,14 @@
       <c r="C101" s="3">
         <v>1</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D101" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E101" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="F101" s="3" t="s">
-        <v>661</v>
+      <c r="F101" s="10" t="s">
+        <v>659</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>130</v>
@@ -7076,14 +7083,14 @@
       <c r="C102" s="3">
         <v>1</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E102" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="F102" s="3" t="s">
-        <v>662</v>
+      <c r="F102" s="10" t="s">
+        <v>660</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>130</v>
@@ -7102,14 +7109,14 @@
       <c r="C103" s="3">
         <v>1</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D103" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E103" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="F103" s="3" t="s">
-        <v>663</v>
+      <c r="F103" s="10" t="s">
+        <v>661</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>130</v>
@@ -7128,14 +7135,14 @@
       <c r="C104" s="3">
         <v>1</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D104" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E104" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="F104" s="3" t="s">
-        <v>664</v>
+      <c r="F104" s="10" t="s">
+        <v>662</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>130</v>
@@ -7146,10 +7153,10 @@
     </row>
     <row r="105" spans="1:9" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E105" s="3" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7162,14 +7169,14 @@
       <c r="C106" s="3">
         <v>1</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E106" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="F106" s="3" t="s">
-        <v>666</v>
+      <c r="F106" s="10" t="s">
+        <v>664</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>130</v>
@@ -7188,14 +7195,14 @@
       <c r="C107" s="3">
         <v>1</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E107" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>667</v>
+      <c r="F107" s="10" t="s">
+        <v>665</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>130</v>
@@ -7206,10 +7213,10 @@
     </row>
     <row r="108" spans="1:9" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E108" s="3" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7222,14 +7229,14 @@
       <c r="C109" s="3">
         <v>1</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="E109" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="F109" s="3" t="s">
-        <v>669</v>
+      <c r="F109" s="10" t="s">
+        <v>667</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>130</v>
@@ -7248,14 +7255,14 @@
       <c r="C110" s="3">
         <v>1</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="E110" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="F110" s="3" t="s">
-        <v>670</v>
+      <c r="F110" s="10" t="s">
+        <v>668</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>130</v>
@@ -7274,14 +7281,14 @@
       <c r="C111" s="3">
         <v>1</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E111" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="F111" s="3" t="s">
-        <v>671</v>
+      <c r="F111" s="10" t="s">
+        <v>669</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>130</v>
@@ -7292,10 +7299,10 @@
     </row>
     <row r="112" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E112" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7308,14 +7315,14 @@
       <c r="C113" s="3">
         <v>1</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D113" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E113" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="F113" s="10" t="s">
-        <v>673</v>
+      <c r="F113" s="11" t="s">
+        <v>671</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>130</v>
@@ -7334,14 +7341,14 @@
       <c r="C114" s="3">
         <v>1</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D114" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="E114" s="3" t="s">
+      <c r="E114" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="F114" s="3" t="s">
-        <v>674</v>
+      <c r="F114" s="10" t="s">
+        <v>672</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>130</v>
@@ -7360,14 +7367,14 @@
       <c r="C115" s="3">
         <v>1</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D115" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="E115" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="F115" s="3" t="s">
-        <v>675</v>
+      <c r="F115" s="10" t="s">
+        <v>673</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>130</v>
@@ -7386,14 +7393,14 @@
       <c r="C116" s="3">
         <v>1</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D116" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="E116" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="F116" s="3" t="s">
-        <v>676</v>
+      <c r="F116" s="10" t="s">
+        <v>674</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>130</v>
@@ -7412,14 +7419,14 @@
       <c r="C117" s="3">
         <v>1</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D117" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E117" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="F117" s="3" t="s">
-        <v>677</v>
+      <c r="F117" s="10" t="s">
+        <v>675</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>130</v>
@@ -7438,14 +7445,14 @@
       <c r="C118" s="3">
         <v>1</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="E118" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="F118" s="3" t="s">
-        <v>678</v>
+      <c r="F118" s="10" t="s">
+        <v>676</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>130</v>
@@ -7464,14 +7471,14 @@
       <c r="C119" s="3">
         <v>1</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D119" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E119" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="F119" s="3" t="s">
-        <v>679</v>
+      <c r="F119" s="10" t="s">
+        <v>677</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>130</v>
@@ -7490,14 +7497,14 @@
       <c r="C120" s="3">
         <v>1</v>
       </c>
-      <c r="D120" s="3" t="s">
+      <c r="D120" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="E120" s="3" t="s">
+      <c r="E120" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="F120" s="3" t="s">
-        <v>680</v>
+      <c r="F120" s="10" t="s">
+        <v>678</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>130</v>
@@ -7516,14 +7523,14 @@
       <c r="C121" s="3">
         <v>1</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="E121" s="3" t="s">
+      <c r="E121" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="F121" s="3" t="s">
-        <v>681</v>
+      <c r="F121" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="H121" s="3" t="s">
         <v>130</v>
@@ -7542,14 +7549,14 @@
       <c r="C122" s="3">
         <v>1</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="D122" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="E122" s="3" t="s">
+      <c r="E122" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="F122" s="3" t="s">
-        <v>682</v>
+      <c r="F122" s="10" t="s">
+        <v>680</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>130</v>
@@ -7568,14 +7575,14 @@
       <c r="C123" s="3">
         <v>1</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="E123" s="3" t="s">
+      <c r="E123" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="F123" s="3" t="s">
-        <v>683</v>
+      <c r="F123" s="10" t="s">
+        <v>681</v>
       </c>
       <c r="H123" s="3" t="s">
         <v>130</v>
@@ -7586,10 +7593,10 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E124" s="3" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>